<commit_message>
Doing the changes in the xlsx file
</commit_message>
<xml_diff>
--- a/getplaced/static/sample/sample_new_accounts.xlsx
+++ b/getplaced/static/sample/sample_new_accounts.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97557687077584a3/Desktop/project/clean_frame/Clean_Frame/static/sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{9CCD58B9-FCD8-4261-B04A-038682A10018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8ECE5AB-03B4-4930-B25D-189EDB9D4EF4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2F537A1-A26D-4B9C-B7F4-B6F7518AB0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{DB20542C-6F78-464B-875C-C1D6BE86CEA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -39,83 +50,83 @@
     <t>Account Type</t>
   </si>
   <si>
+    <t>CGPA</t>
+  </si>
+  <si>
+    <t>IT2050001</t>
+  </si>
+  <si>
+    <t>it2050001@thapar.edu</t>
+  </si>
+  <si>
     <t>student</t>
   </si>
   <si>
+    <t>IT2050002</t>
+  </si>
+  <si>
+    <t>it2050002@thapar.edu</t>
+  </si>
+  <si>
+    <t>IT2050003</t>
+  </si>
+  <si>
+    <t>it2050003@thapar.edu</t>
+  </si>
+  <si>
+    <t>IT2050004</t>
+  </si>
+  <si>
+    <t>it2050004@thapar.edu</t>
+  </si>
+  <si>
+    <t>IT2050005</t>
+  </si>
+  <si>
+    <t>it2050005@thapar.edu</t>
+  </si>
+  <si>
+    <t>Company 1</t>
+  </si>
+  <si>
+    <t>email 1</t>
+  </si>
+  <si>
     <t>company</t>
   </si>
   <si>
-    <t>IIT2050001</t>
-  </si>
-  <si>
-    <t>IIT2050002</t>
-  </si>
-  <si>
-    <t>IIT2050003</t>
-  </si>
-  <si>
-    <t>IIT2050004</t>
-  </si>
-  <si>
-    <t>IIT2050005</t>
-  </si>
-  <si>
-    <t>iit2050001@iiita.ac.in</t>
-  </si>
-  <si>
-    <t>iit2050002@iiita.ac.in</t>
-  </si>
-  <si>
-    <t>iit2050003@iiita.ac.in</t>
-  </si>
-  <si>
-    <t>iit2050004@iiita.ac.in</t>
-  </si>
-  <si>
-    <t>iit2050005@iiita.ac.in</t>
-  </si>
-  <si>
-    <t>Company 1</t>
+    <t>NaN</t>
   </si>
   <si>
     <t>Company 2</t>
   </si>
   <si>
+    <t>email 2</t>
+  </si>
+  <si>
     <t>Company 3</t>
   </si>
   <si>
+    <t>email 3</t>
+  </si>
+  <si>
     <t>Company 4</t>
   </si>
   <si>
+    <t>email 4</t>
+  </si>
+  <si>
     <t>Company 5</t>
   </si>
   <si>
-    <t>email 1</t>
-  </si>
-  <si>
-    <t>email 2</t>
-  </si>
-  <si>
-    <t>email 3</t>
-  </si>
-  <si>
-    <t>email 4</t>
-  </si>
-  <si>
     <t>email 5</t>
-  </si>
-  <si>
-    <t>CGPA</t>
-  </si>
-  <si>
-    <t>NaN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -474,17 +485,17 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="29.5703125" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -498,95 +509,95 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E2">
         <v>7.8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
       </c>
       <c r="E3">
         <v>9.23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E4">
         <v>7.87</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E5">
         <v>8.31</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E6">
         <v>8.6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -594,78 +605,78 @@
         <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="C13" s="1"/>
     </row>
   </sheetData>

</xml_diff>